<commit_message>
Large Excel file parsing workin :)
</commit_message>
<xml_diff>
--- a/src/test/resources/com/nach/core/testfiles/excel/medium-file-for-excel-test.xlsx
+++ b/src/test/resources/com/nach/core/testfiles/excel/medium-file-for-excel-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_WORKSPACES\_ECLIPSE_WORKSPACE\workspace\core\src\test\resources\com\nach\core\testfiles\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8AF3C8-93CF-46B6-A9E9-513432567093}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5FA96B-589F-48A1-9A23-BA17F85F4DE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00031EB1-E0C6-40AE-9A6C-A9DA0D8C8B89}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00031EB1-E0C6-40AE-9A6C-A9DA0D8C8B89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20674" uniqueCount="1239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20676" uniqueCount="1241">
   <si>
     <t>Patient_ID</t>
   </si>
@@ -3750,6 +3750,12 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>smith</t>
+  </si>
+  <si>
+    <t>jones</t>
   </si>
 </sst>
 </file>
@@ -3785,9 +3791,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4102,7 +4109,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57225FE-9D09-4BB2-8FBE-26F6309C4F47}">
-  <dimension ref="A1:AUN17"/>
+  <dimension ref="A1:AUN21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -67208,7 +67215,40 @@
         <v>1237</v>
       </c>
     </row>
+    <row r="18" spans="1:1236" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>123</v>
+      </c>
+      <c r="B18" s="2">
+        <v>43550</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1236" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B19" s="2">
+        <v>43550</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1236" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B20" s="2">
+        <v>43550</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1236" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>43550</v>
+      </c>
+      <c r="B21">
+        <v>43550</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>